<commit_message>
Added new plotting, removed some redundant code
</commit_message>
<xml_diff>
--- a/cell_numbers_for_model.xlsx
+++ b/cell_numbers_for_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niall\Documents\MPhys\Systems-Medicine-for-Chronic-Kidney-Disease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB86149-C14A-4E19-B451-4A4CD7038399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12D4FFD-98F3-404D-9427-500CCC8BA7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4648CF15-1519-402A-AD70-36A8F253368D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{4648CF15-1519-402A-AD70-36A8F253368D}"/>
   </bookViews>
   <sheets>
     <sheet name="cell_numbers_for_model" sheetId="1" r:id="rId1"/>
@@ -950,12 +950,12 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -978,7 +978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6</v>
       </c>

</xml_diff>